<commit_message>
edits to main timeline
</commit_message>
<xml_diff>
--- a/bl_arduinoController/data/bl_timelinenotes_excel.xlsx
+++ b/bl_arduinoController/data/bl_timelinenotes_excel.xlsx
@@ -29,9 +29,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="0.000"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -190,7 +189,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -219,12 +218,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1309,14 +1302,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:C40"/>
+  <dimension ref="A2:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7188" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.35156" style="1" customWidth="1"/>
     <col min="4" max="256" width="8.35156" style="1" customWidth="1"/>
   </cols>
@@ -1341,21 +1334,21 @@
     </row>
     <row r="3" ht="20.25" customHeight="1">
       <c r="A3" s="4">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B3" s="5">
-        <v>408</v>
+        <v>0</v>
       </c>
       <c r="C3" s="6">
-        <v>270</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
       <c r="A4" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="8">
-        <v>459.6</v>
+        <v>408</v>
       </c>
       <c r="C4" s="9">
         <v>270</v>
@@ -1363,10 +1356,10 @@
     </row>
     <row r="5" ht="20.05" customHeight="1">
       <c r="A5" s="7">
-        <v>6</v>
-      </c>
-      <c r="B5" s="10">
-        <v>1042.56</v>
+        <v>2</v>
+      </c>
+      <c r="B5" s="8">
+        <v>459.6</v>
       </c>
       <c r="C5" s="9">
         <v>270</v>
@@ -1376,8 +1369,8 @@
       <c r="A6" s="7">
         <v>6</v>
       </c>
-      <c r="B6" s="11">
-        <v>1059.6</v>
+      <c r="B6" s="8">
+        <v>862.5599999999999</v>
       </c>
       <c r="C6" s="9">
         <v>270</v>
@@ -1385,76 +1378,76 @@
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" s="7">
-        <v>12</v>
-      </c>
-      <c r="B7" s="10">
-        <v>1061.7</v>
+        <v>6</v>
+      </c>
+      <c r="B7" s="8">
+        <v>879.6</v>
       </c>
       <c r="C7" s="9">
-        <v>100</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" s="7">
-        <v>8</v>
-      </c>
-      <c r="B8" s="10">
-        <v>1070.22</v>
+        <v>12</v>
+      </c>
+      <c r="B8" s="8">
+        <v>881.7</v>
       </c>
       <c r="C8" s="9">
-        <v>270</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" s="7">
-        <v>13</v>
-      </c>
-      <c r="B9" s="10">
-        <v>1097.04</v>
+        <v>8</v>
+      </c>
+      <c r="B9" s="8">
+        <v>890.22</v>
       </c>
       <c r="C9" s="9">
-        <v>270</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" s="7">
-        <v>5</v>
-      </c>
-      <c r="B10" s="10">
-        <v>1102.14</v>
+        <v>13</v>
+      </c>
+      <c r="B10" s="8">
+        <v>917.04</v>
       </c>
       <c r="C10" s="9">
-        <v>270</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" s="7">
-        <v>9</v>
-      </c>
-      <c r="B11" s="10">
-        <v>1110.66</v>
+        <v>5</v>
+      </c>
+      <c r="B11" s="8">
+        <v>922.14</v>
       </c>
       <c r="C11" s="9">
-        <v>270</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" s="7">
-        <v>3</v>
-      </c>
-      <c r="B12" s="10">
-        <v>1110.66</v>
+        <v>9</v>
+      </c>
+      <c r="B12" s="8">
+        <v>930.66</v>
       </c>
       <c r="C12" s="9">
-        <v>270</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" s="7">
-        <v>5</v>
-      </c>
-      <c r="B13" s="10">
-        <v>1123.38</v>
+        <v>3</v>
+      </c>
+      <c r="B13" s="8">
+        <v>930.66</v>
       </c>
       <c r="C13" s="9">
         <v>100</v>
@@ -1464,8 +1457,8 @@
       <c r="A14" s="7">
         <v>5</v>
       </c>
-      <c r="B14" s="10">
-        <v>1129.38</v>
+      <c r="B14" s="8">
+        <v>943.38</v>
       </c>
       <c r="C14" s="9">
         <v>100</v>
@@ -1475,8 +1468,8 @@
       <c r="A15" s="7">
         <v>5</v>
       </c>
-      <c r="B15" s="10">
-        <v>1135.38</v>
+      <c r="B15" s="8">
+        <v>949.38</v>
       </c>
       <c r="C15" s="9">
         <v>100</v>
@@ -1486,8 +1479,8 @@
       <c r="A16" s="7">
         <v>5</v>
       </c>
-      <c r="B16" s="10">
-        <v>1141.38</v>
+      <c r="B16" s="8">
+        <v>955.38</v>
       </c>
       <c r="C16" s="9">
         <v>100</v>
@@ -1495,21 +1488,21 @@
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" s="7">
-        <v>7</v>
-      </c>
-      <c r="B17" s="10">
-        <v>1148.94</v>
+        <v>5</v>
+      </c>
+      <c r="B17" s="8">
+        <v>961.38</v>
       </c>
       <c r="C17" s="9">
-        <v>270</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" s="7">
-        <v>8</v>
-      </c>
-      <c r="B18" s="10">
-        <v>1165.98</v>
+        <v>7</v>
+      </c>
+      <c r="B18" s="8">
+        <v>968.9400000000001</v>
       </c>
       <c r="C18" s="9">
         <v>270</v>
@@ -1517,153 +1510,153 @@
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" s="7">
-        <v>4</v>
-      </c>
-      <c r="B19" s="10">
-        <v>1168.08</v>
+        <v>8</v>
+      </c>
+      <c r="B19" s="8">
+        <v>985.98</v>
       </c>
       <c r="C19" s="9">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" ht="20.05" customHeight="1">
       <c r="A20" s="7">
         <v>4</v>
       </c>
-      <c r="B20" s="10">
-        <v>1187.22</v>
+      <c r="B20" s="8">
+        <v>988.08</v>
       </c>
       <c r="C20" s="9">
-        <v>270</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" s="7">
-        <v>8</v>
-      </c>
-      <c r="B21" s="10">
-        <v>1212.78</v>
+        <v>4</v>
+      </c>
+      <c r="B21" s="8">
+        <v>1007.22</v>
       </c>
       <c r="C21" s="9">
-        <v>270</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" s="7">
-        <v>7</v>
-      </c>
-      <c r="B22" s="10">
-        <v>1212.78</v>
+        <v>8</v>
+      </c>
+      <c r="B22" s="8">
+        <v>1032.78</v>
       </c>
       <c r="C22" s="9">
-        <v>270</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" s="7">
-        <v>12</v>
-      </c>
-      <c r="B23" s="10">
-        <v>1353.18</v>
+        <v>7</v>
+      </c>
+      <c r="B23" s="8">
+        <v>1032.78</v>
       </c>
       <c r="C23" s="9">
-        <v>270</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" s="7">
-        <v>10</v>
-      </c>
-      <c r="B24" s="10">
-        <v>1378.74</v>
+        <v>12</v>
+      </c>
+      <c r="B24" s="8">
+        <v>1173.18</v>
       </c>
       <c r="C24" s="9">
-        <v>270</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" ht="20.05" customHeight="1">
       <c r="A25" s="7">
-        <v>11</v>
-      </c>
-      <c r="B25" s="10">
-        <v>1385.1</v>
+        <v>10</v>
+      </c>
+      <c r="B25" s="8">
+        <v>1198.74</v>
       </c>
       <c r="C25" s="9">
-        <v>270</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" ht="20.05" customHeight="1">
       <c r="A26" s="7">
-        <v>12</v>
-      </c>
-      <c r="B26" s="10">
-        <v>1404.24</v>
+        <v>11</v>
+      </c>
+      <c r="B26" s="8">
+        <v>1205.1</v>
       </c>
       <c r="C26" s="9">
-        <v>270</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" ht="20.05" customHeight="1">
       <c r="A27" s="7">
         <v>12</v>
       </c>
-      <c r="B27" s="10">
-        <v>1417.02</v>
+      <c r="B27" s="8">
+        <v>1224.24</v>
       </c>
       <c r="C27" s="9">
-        <v>270</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" ht="20.05" customHeight="1">
       <c r="A28" s="7">
         <v>12</v>
       </c>
-      <c r="B28" s="10">
-        <v>1436.16</v>
+      <c r="B28" s="8">
+        <v>1237.02</v>
       </c>
       <c r="C28" s="9">
-        <v>270</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" ht="20.05" customHeight="1">
       <c r="A29" s="7">
-        <v>10</v>
-      </c>
-      <c r="B29" s="10">
-        <v>1455.3</v>
+        <v>12</v>
+      </c>
+      <c r="B29" s="8">
+        <v>1256.16</v>
       </c>
       <c r="C29" s="9">
-        <v>270</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" ht="20.05" customHeight="1">
       <c r="A30" s="7">
-        <v>8</v>
-      </c>
-      <c r="B30" s="10">
-        <v>1493.64</v>
+        <v>10</v>
+      </c>
+      <c r="B30" s="8">
+        <v>1275.3</v>
       </c>
       <c r="C30" s="9">
-        <v>270</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" ht="20.05" customHeight="1">
       <c r="A31" s="7">
         <v>8</v>
       </c>
-      <c r="B31" s="10">
-        <v>1736.16</v>
+      <c r="B31" s="8">
+        <v>1313.64</v>
       </c>
       <c r="C31" s="9">
-        <v>100</v>
+        <v>270</v>
       </c>
     </row>
     <row r="32" ht="20.05" customHeight="1">
       <c r="A32" s="7">
-        <v>13</v>
-      </c>
-      <c r="B32" s="10">
-        <v>1736.16</v>
+        <v>8</v>
+      </c>
+      <c r="B32" s="8">
+        <v>1556.16</v>
       </c>
       <c r="C32" s="9">
         <v>100</v>
@@ -1671,89 +1664,100 @@
     </row>
     <row r="33" ht="20.05" customHeight="1">
       <c r="A33" s="7">
-        <v>15</v>
-      </c>
-      <c r="B33" s="10">
-        <v>1748.94</v>
+        <v>13</v>
+      </c>
+      <c r="B33" s="8">
+        <v>1556.16</v>
       </c>
       <c r="C33" s="9">
-        <v>270</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" ht="20.05" customHeight="1">
       <c r="A34" s="7">
-        <v>12</v>
-      </c>
-      <c r="B34" s="10">
-        <v>1876.62</v>
+        <v>15</v>
+      </c>
+      <c r="B34" s="8">
+        <v>1568.94</v>
       </c>
       <c r="C34" s="9">
-        <v>270</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" ht="20.05" customHeight="1">
       <c r="A35" s="7">
-        <v>5</v>
-      </c>
-      <c r="B35" s="10">
-        <v>2182.98</v>
+        <v>12</v>
+      </c>
+      <c r="B35" s="8">
+        <v>1696.62</v>
       </c>
       <c r="C35" s="9">
-        <v>270</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" ht="20.05" customHeight="1">
       <c r="A36" s="7">
-        <v>14</v>
-      </c>
-      <c r="B36" s="10">
-        <v>2278.74</v>
+        <v>5</v>
+      </c>
+      <c r="B36" s="8">
+        <v>2002.98</v>
       </c>
       <c r="C36" s="9">
-        <v>270</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" ht="20.05" customHeight="1">
       <c r="A37" s="7">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B37" s="8">
-        <v>2400</v>
+        <v>2098.74</v>
       </c>
       <c r="C37" s="9">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" ht="20.05" customHeight="1">
       <c r="A38" s="7">
-        <v>4</v>
-      </c>
-      <c r="B38" s="10">
-        <v>2425.56</v>
+        <v>3</v>
+      </c>
+      <c r="B38" s="8">
+        <v>2220</v>
       </c>
       <c r="C38" s="9">
-        <v>270</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" ht="20.05" customHeight="1">
       <c r="A39" s="7">
-        <v>12</v>
-      </c>
-      <c r="B39" s="10">
-        <v>2636.16</v>
+        <v>4</v>
+      </c>
+      <c r="B39" s="8">
+        <v>2245.56</v>
       </c>
       <c r="C39" s="9">
-        <v>270</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" ht="20.05" customHeight="1">
       <c r="A40" s="7">
+        <v>12</v>
+      </c>
+      <c r="B40" s="8">
+        <v>2456.16</v>
+      </c>
+      <c r="C40" s="9">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="41" ht="20.05" customHeight="1">
+      <c r="A41" s="7">
         <v>9</v>
       </c>
-      <c r="B40" s="8">
-        <v>3600</v>
-      </c>
-      <c r="C40" s="9">
+      <c r="B41" s="8">
+        <v>3060</v>
+      </c>
+      <c r="C41" s="9">
         <v>270</v>
       </c>
     </row>

</xml_diff>